<commit_message>
Mise à jour Backlog Product
J'ai mis à jour le backlog product
</commit_message>
<xml_diff>
--- a/OUT OF BOUNDS - Conception/Backlog Product.xlsx
+++ b/OUT OF BOUNDS - Conception/Backlog Product.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\OneDrive\Bureau\GitHub\CryptOfTheJavaDancer\OUT OF BOUNDS - Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FD0607-CBA9-49B4-8E78-0C8D5774E7D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0575A93-308E-4C1B-8C5E-35977F765695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{76DF5FBA-9E68-4B72-AD7F-372E7DDAABA9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="320">
   <si>
     <t>Fonctionnalités mères</t>
   </si>
@@ -990,6 +990,9 @@
   </si>
   <si>
     <t>17.7</t>
+  </si>
+  <si>
+    <t>Terminé</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1123,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1317,6 +1320,21 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1332,22 +1350,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1680,7 +1683,7 @@
   <dimension ref="A1:O157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,39 +1697,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
     </row>
     <row r="6" spans="1:15" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1769,7 +1772,7 @@
         <v>26</v>
       </c>
       <c r="G9" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1786,7 +1789,7 @@
         <v>59</v>
       </c>
       <c r="G10" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1803,7 +1806,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1820,7 +1823,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1837,7 +1840,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1858,7 +1861,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1875,7 +1878,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1892,7 +1895,7 @@
         <v>66</v>
       </c>
       <c r="G16" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1909,7 +1912,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1925,8 +1928,8 @@
       <c r="F18" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>9</v>
+      <c r="G18" s="60" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1969,8 +1972,8 @@
       <c r="F20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>9</v>
+      <c r="G20" s="60" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1986,8 +1989,8 @@
       <c r="F21" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>9</v>
+      <c r="G21" s="60" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2003,8 +2006,8 @@
       <c r="F22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>9</v>
+      <c r="G22" s="60" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2025,7 +2028,7 @@
         <v>23</v>
       </c>
       <c r="G23" s="61" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2042,7 +2045,7 @@
         <v>24</v>
       </c>
       <c r="G24" s="60" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2059,7 +2062,7 @@
         <v>25</v>
       </c>
       <c r="G25" s="62" t="s">
-        <v>9</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2104,8 +2107,8 @@
       <c r="F27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>9</v>
+      <c r="G27" s="60" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2401,12 +2404,12 @@
         <v>43</v>
       </c>
       <c r="C48" s="16"/>
-      <c r="D48" s="59" t="s">
+      <c r="D48" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -2450,12 +2453,12 @@
         <v>45</v>
       </c>
       <c r="C51" s="47"/>
-      <c r="D51" s="56" t="s">
+      <c r="D51" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
@@ -2499,12 +2502,12 @@
         <v>51</v>
       </c>
       <c r="C54" s="16"/>
-      <c r="D54" s="59" t="s">
+      <c r="D54" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="59"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="52"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
@@ -2548,12 +2551,12 @@
         <v>55</v>
       </c>
       <c r="C57" s="47"/>
-      <c r="D57" s="56" t="s">
+      <c r="D57" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="E57" s="56"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="56"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
@@ -2654,12 +2657,12 @@
         <v>63</v>
       </c>
       <c r="C63" s="14"/>
-      <c r="D63" s="56" t="s">
+      <c r="D63" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -3339,12 +3342,12 @@
         <v>43</v>
       </c>
       <c r="C105" s="26"/>
-      <c r="D105" s="52" t="s">
+      <c r="D105" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="E105" s="52"/>
-      <c r="F105" s="52"/>
-      <c r="G105" s="52"/>
+      <c r="E105" s="57"/>
+      <c r="F105" s="57"/>
+      <c r="G105" s="57"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="23">
@@ -3354,12 +3357,12 @@
         <v>45</v>
       </c>
       <c r="C106" s="23"/>
-      <c r="D106" s="55" t="s">
+      <c r="D106" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="E106" s="55"/>
-      <c r="F106" s="55"/>
-      <c r="G106" s="55"/>
+      <c r="E106" s="59"/>
+      <c r="F106" s="59"/>
+      <c r="G106" s="59"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="26">
@@ -3369,12 +3372,12 @@
         <v>51</v>
       </c>
       <c r="C107" s="26"/>
-      <c r="D107" s="52" t="s">
+      <c r="D107" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="E107" s="52"/>
-      <c r="F107" s="52"/>
-      <c r="G107" s="52"/>
+      <c r="E107" s="57"/>
+      <c r="F107" s="57"/>
+      <c r="G107" s="57"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="23">
@@ -3384,12 +3387,12 @@
         <v>55</v>
       </c>
       <c r="C108" s="23"/>
-      <c r="D108" s="55" t="s">
+      <c r="D108" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="E108" s="55"/>
-      <c r="F108" s="55"/>
-      <c r="G108" s="55"/>
+      <c r="E108" s="59"/>
+      <c r="F108" s="59"/>
+      <c r="G108" s="59"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="26">
@@ -3589,12 +3592,12 @@
         <v>126</v>
       </c>
       <c r="C119" s="39"/>
-      <c r="D119" s="49" t="s">
+      <c r="D119" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="E119" s="50"/>
-      <c r="F119" s="50"/>
-      <c r="G119" s="51"/>
+      <c r="E119" s="55"/>
+      <c r="F119" s="55"/>
+      <c r="G119" s="56"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
@@ -3782,12 +3785,12 @@
       <c r="C130" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="D130" s="49" t="s">
+      <c r="D130" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="E130" s="50"/>
-      <c r="F130" s="50"/>
-      <c r="G130" s="51"/>
+      <c r="E130" s="55"/>
+      <c r="F130" s="55"/>
+      <c r="G130" s="56"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
@@ -4083,12 +4086,12 @@
       <c r="C147" s="26" t="s">
         <v>318</v>
       </c>
-      <c r="D147" s="52" t="s">
+      <c r="D147" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="E147" s="52"/>
-      <c r="F147" s="52"/>
-      <c r="G147" s="52"/>
+      <c r="E147" s="57"/>
+      <c r="F147" s="57"/>
+      <c r="G147" s="57"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
@@ -4260,11 +4263,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="H1:O2"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D51:G51"/>
-    <mergeCell ref="D54:G54"/>
     <mergeCell ref="D130:G130"/>
     <mergeCell ref="D119:G119"/>
     <mergeCell ref="D147:G147"/>
@@ -4275,6 +4273,11 @@
     <mergeCell ref="D105:G105"/>
     <mergeCell ref="D106:G106"/>
     <mergeCell ref="D107:G107"/>
+    <mergeCell ref="H1:O2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="D54:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>